<commit_message>
updated program so that overlay of spectra works correctly
</commit_message>
<xml_diff>
--- a/exampleProblems/JAI_234A/JAI_234A.xlsx
+++ b/exampleProblems/JAI_234A/JAI_234A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/JAI_234A/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_1FE4DB5A60BCE47852A46819C3F7C22B33F682DB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5DC229E-371A-4330-BFA1-F24B57E84EC8}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_09728AAD2F266361EE4B7A32AF1BF046A376A3B5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF08AAF-0CF9-2F43-823B-02867A43CD15}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="990" windowWidth="20295" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7280" yWindow="1000" windowWidth="20300" windowHeight="13620" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="COSY" sheetId="5" r:id="rId5"/>
     <sheet name="HSQC" sheetId="6" r:id="rId6"/>
     <sheet name="HMBC" sheetId="7" r:id="rId7"/>
+    <sheet name="NOESY" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="190">
   <si>
     <t>molecule</t>
   </si>
@@ -602,7 +603,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1111,13 +1112,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1130,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1149,9 +1154,9 @@
       <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -1178,7 +1183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1207,7 +1212,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1236,7 +1241,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1265,7 +1270,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1294,7 +1299,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1323,7 +1328,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="1"/>
     </row>
   </sheetData>
@@ -1340,9 +1345,9 @@
       <selection sqref="A1:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1368,7 +1373,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1391,7 +1396,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1414,7 +1419,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1437,7 +1442,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1460,7 +1465,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1483,7 +1488,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1506,7 +1511,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1529,7 +1534,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1552,7 +1557,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1588,9 +1593,9 @@
       <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1616,7 +1621,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1639,7 +1644,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1662,7 +1667,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1685,7 +1690,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1708,7 +1713,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1741,12 +1746,12 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>90</v>
       </c>
@@ -1778,7 +1783,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1807,7 +1812,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1849,9 +1854,9 @@
       <selection sqref="A1:K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>90</v>
       </c>
@@ -1883,7 +1888,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1912,7 +1917,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1941,7 +1946,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1970,7 +1975,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1999,7 +2004,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2041,9 +2046,9 @@
       <selection sqref="A1:K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="B1" s="1" t="s">
         <v>90</v>
       </c>
@@ -2075,7 +2080,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2104,7 +2109,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2133,7 +2138,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2162,7 +2167,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2191,7 +2196,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2220,7 +2225,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2249,7 +2254,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2278,7 +2283,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2307,7 +2312,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2336,7 +2341,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2365,7 +2370,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2394,7 +2399,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2423,7 +2428,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2452,7 +2457,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2481,7 +2486,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2508,6 +2513,53 @@
       </c>
       <c r="I16" t="s">
         <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD7213D-38B6-6E4F-B0BB-20A702A0C646}">
+  <dimension ref="B1:K1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:11">
+      <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more checks when reading in from excel
</commit_message>
<xml_diff>
--- a/exampleProblems/JAI_234A/JAI_234A.xlsx
+++ b/exampleProblems/JAI_234A/JAI_234A.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/JAI_234A/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_09728AAD2F266361EE4B7A32AF1BF046A376A3B5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF08AAF-0CF9-2F43-823B-02867A43CD15}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="11_09728AAD2F266361EE4B7A32AF1BF046A376A3B5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47CF149A-A332-4F34-BE72-93E2C1D95CB0}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="1000" windowWidth="20300" windowHeight="13620" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="183">
   <si>
     <t>molecule</t>
   </si>
@@ -359,9 +359,6 @@
     <t>26.53</t>
   </si>
   <si>
-    <t>-0.5</t>
-  </si>
-  <si>
     <t>4.8</t>
   </si>
   <si>
@@ -404,9 +401,6 @@
     <t>53.43</t>
   </si>
   <si>
-    <t>-0.56</t>
-  </si>
-  <si>
     <t>33.84</t>
   </si>
   <si>
@@ -422,25 +416,10 @@
     <t>6.19</t>
   </si>
   <si>
-    <t>101.15</t>
-  </si>
-  <si>
     <t>162.66</t>
   </si>
   <si>
-    <t>110.47</t>
-  </si>
-  <si>
-    <t>151.07</t>
-  </si>
-  <si>
-    <t>168.87</t>
-  </si>
-  <si>
     <t>100.78</t>
-  </si>
-  <si>
-    <t>109.86</t>
   </si>
   <si>
     <t>103.83</t>
@@ -603,7 +582,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1116,21 +1095,21 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1138,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1151,12 +1130,12 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I6"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>2</v>
@@ -1183,7 +1162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1212,7 +1191,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1241,7 +1220,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1270,7 +1249,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1299,7 +1278,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -1328,7 +1307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
   </sheetData>
@@ -1342,12 +1321,12 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:I10"/>
+      <selection activeCell="B2" sqref="B2:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1373,7 +1352,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1396,7 +1375,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1419,7 +1398,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1442,7 +1421,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1465,7 +1444,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1488,7 +1467,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1511,7 +1490,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1534,7 +1513,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1557,7 +1536,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1593,9 +1572,9 @@
       <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1621,7 +1600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1644,7 +1623,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1667,7 +1646,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1690,7 +1669,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1713,7 +1692,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1749,9 +1728,9 @@
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>90</v>
       </c>
@@ -1783,7 +1762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1812,7 +1791,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1851,12 +1830,12 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>90</v>
       </c>
@@ -1888,7 +1867,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1898,17 +1877,17 @@
       <c r="C2" t="s">
         <v>105</v>
       </c>
-      <c r="D2" t="s">
-        <v>110</v>
+      <c r="D2">
+        <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G2" t="s">
-        <v>125</v>
+        <v>119</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
       </c>
       <c r="H2" t="s">
         <v>74</v>
@@ -1917,7 +1896,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1928,16 +1907,16 @@
         <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H3" t="s">
         <v>74</v>
@@ -1946,7 +1925,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1957,16 +1936,16 @@
         <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H4" t="s">
         <v>74</v>
@@ -1975,7 +1954,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1986,16 +1965,16 @@
         <v>108</v>
       </c>
       <c r="D5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H5" t="s">
         <v>74</v>
@@ -2004,7 +1983,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2015,16 +1994,16 @@
         <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H6" t="s">
         <v>74</v>
@@ -2042,13 +2021,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>90</v>
       </c>
@@ -2080,7 +2059,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2088,19 +2067,19 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
         <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="G2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="H2" t="s">
         <v>74</v>
@@ -2109,7 +2088,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2117,19 +2096,19 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F3" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G3" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="H3" t="s">
         <v>74</v>
@@ -2138,7 +2117,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2146,19 +2125,19 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>96</v>
       </c>
       <c r="E4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F4" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="G4" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="H4" t="s">
         <v>74</v>
@@ -2167,7 +2146,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2175,19 +2154,19 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
         <v>96</v>
       </c>
       <c r="E5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="G5" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H5" t="s">
         <v>74</v>
@@ -2195,8 +2174,9 @@
       <c r="I5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2204,19 +2184,19 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D6" t="s">
         <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="G6" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H6" t="s">
         <v>74</v>
@@ -2224,8 +2204,9 @@
       <c r="I6" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2233,19 +2214,19 @@
         <v>76</v>
       </c>
       <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
         <v>136</v>
       </c>
-      <c r="D7" t="s">
-        <v>143</v>
-      </c>
       <c r="E7" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F7" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="G7" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="H7" t="s">
         <v>74</v>
@@ -2253,8 +2234,9 @@
       <c r="I7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2262,19 +2244,19 @@
         <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
         <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="G8" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H8" t="s">
         <v>74</v>
@@ -2282,28 +2264,29 @@
       <c r="I8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F9" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="G9" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H9" t="s">
         <v>74</v>
@@ -2311,8 +2294,9 @@
       <c r="I9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2320,19 +2304,19 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F10" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G10" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H10" t="s">
         <v>74</v>
@@ -2341,7 +2325,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2349,19 +2333,19 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" t="s">
         <v>138</v>
       </c>
-      <c r="D11" t="s">
-        <v>145</v>
-      </c>
       <c r="E11" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F11" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="G11" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H11" t="s">
         <v>74</v>
@@ -2370,7 +2354,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2378,19 +2362,19 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D12" t="s">
         <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F12" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G12" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="H12" t="s">
         <v>74</v>
@@ -2399,7 +2383,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2407,19 +2391,19 @@
         <v>103</v>
       </c>
       <c r="C13" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E13" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F13" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G13" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="H13" t="s">
         <v>74</v>
@@ -2428,7 +2412,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2436,19 +2420,19 @@
         <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E14" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F14" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G14" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="H14" t="s">
         <v>74</v>
@@ -2457,7 +2441,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2465,19 +2449,19 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D15" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E15" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F15" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G15" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="H15" t="s">
         <v>74</v>
@@ -2486,7 +2470,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2494,19 +2478,19 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E16" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F16" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G16" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="H16" t="s">
         <v>74</v>
@@ -2524,13 +2508,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD7213D-38B6-6E4F-B0BB-20A702A0C646}">
   <dimension ref="B1:K1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>90</v>
       </c>

</xml_diff>